<commit_message>
concept maps imuno e ealergias
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Imunizacao/ConceptMap/brimunobiogico-sct.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Imunizacao/ConceptMap/brimunobiogico-sct.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Entregaveis/1.RepositorioSemantico/Imunizacao/ConceptMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8862041-878B-104F-9EAF-22BB7EB4D5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8AEEBE-50B7-4B45-ADC6-E520CF9BD8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="1080" windowWidth="24840" windowHeight="13440" xr2:uid="{F59DAF0E-B1FE-DC47-A5F4-187CB422FD94}"/>
+    <workbookView xWindow="8440" yWindow="760" windowWidth="24840" windowHeight="13440" xr2:uid="{F59DAF0E-B1FE-DC47-A5F4-187CB422FD94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$K$1:$K$76</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1137,11 +1137,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F248D098-89B3-CC41-B3AD-EB932F8A3134}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:XFD77"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="8" max="8" width="33" customWidth="1"/>
+    <col min="11" max="11" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
mapas de conceito cbara e imunizacao
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Imunizacao/ConceptMap/brimunobiogico-sct.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Imunizacao/ConceptMap/brimunobiogico-sct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Entregaveis/1.RepositorioSemantico/Imunizacao/ConceptMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E05F378-4EA6-A34A-8F04-E87E5FA660B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80A6E85-FDD0-DE4F-9D6D-0EDF97BAE218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1400" windowWidth="24840" windowHeight="13440" xr2:uid="{F59DAF0E-B1FE-DC47-A5F4-187CB422FD94}"/>
+    <workbookView xWindow="880" yWindow="1400" windowWidth="27380" windowHeight="15860" xr2:uid="{F59DAF0E-B1FE-DC47-A5F4-187CB422FD94}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapeamento" sheetId="1" r:id="rId1"/>
@@ -822,6 +822,23 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -839,23 +856,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1174,13 +1174,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F248D098-89B3-CC41-B3AD-EB932F8A3134}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
@@ -2862,19 +2863,19 @@
       </c>
     </row>
     <row r="46" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" s="18">
+      <c r="A46" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="25">
         <v>70</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" s="20" t="s">
+      <c r="D46" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="27" t="s">
         <v>22</v>
       </c>
       <c r="F46" s="7" t="s">
@@ -2900,11 +2901,11 @@
       </c>
     </row>
     <row r="47" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="21"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="28"/>
       <c r="F47" s="7" t="s">
         <v>7</v>
       </c>
@@ -3875,84 +3876,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="16" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="21">
         <v>3</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="18">
         <f>3/99</f>
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="23">
+      <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="21">
         <v>32</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="18">
         <f>B3/99</f>
         <v>0.32323232323232326</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="23">
+      <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="21">
         <v>0</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="23">
+      <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="21">
         <v>40</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="18">
         <f>B5/99</f>
         <v>0.40404040404040403</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="23">
-        <v>5</v>
-      </c>
-      <c r="B6" s="27">
+      <c r="A6" s="17">
+        <v>5</v>
+      </c>
+      <c r="B6" s="21">
         <v>24</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="18">
         <f>B6/99</f>
         <v>0.24242424242424243</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="22">
         <f>SUM(B2:B6)</f>
         <v>99</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="18">
         <f>SUM(C2:C6)</f>
         <v>1</v>
       </c>

</xml_diff>